<commit_message>
need to resolve border problem
</commit_message>
<xml_diff>
--- a/routine_final.xlsx
+++ b/routine_final.xlsx
@@ -64,7 +64,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -72,20 +72,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -471,12 +522,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Day</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Year</t>
         </is>
@@ -528,63 +579,77 @@
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>CSE 1100 (Prof. G)</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr"/>
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>CSE 1101 (Prof. H)</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr"/>
-      <c r="G2" s="3" t="inlineStr"/>
-      <c r="H2" s="3" t="inlineStr"/>
-      <c r="I2" s="3" t="inlineStr"/>
+      <c r="F2" s="4" t="inlineStr"/>
+      <c r="G2" s="5" t="n"/>
+      <c r="H2" s="5" t="n"/>
+      <c r="I2" s="5" t="n"/>
     </row>
     <row r="3">
-      <c r="B3" s="4" t="inlineStr">
+      <c r="A3" s="5" t="n"/>
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr"/>
-      <c r="D3" s="3" t="inlineStr"/>
-      <c r="E3" s="3" t="inlineStr"/>
-      <c r="F3" s="3" t="inlineStr"/>
-      <c r="G3" s="3" t="inlineStr"/>
-      <c r="H3" s="3" t="inlineStr"/>
-      <c r="I3" s="3" t="inlineStr"/>
+      <c r="C3" s="4" t="inlineStr"/>
+      <c r="D3" s="5" t="n"/>
+      <c r="E3" s="5" t="n"/>
+      <c r="F3" s="5" t="n"/>
+      <c r="G3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
+      <c r="I3" s="5" t="n"/>
     </row>
     <row r="4">
-      <c r="B4" s="5" t="inlineStr">
+      <c r="A4" s="5" t="n"/>
+      <c r="B4" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr"/>
-      <c r="D4" s="3" t="inlineStr"/>
-      <c r="E4" s="3" t="inlineStr"/>
-      <c r="F4" s="3" t="inlineStr"/>
-      <c r="G4" s="3" t="inlineStr"/>
-      <c r="H4" s="3" t="inlineStr"/>
-      <c r="I4" s="3" t="inlineStr"/>
+      <c r="C4" s="4" t="inlineStr"/>
+      <c r="D4" s="5" t="n"/>
+      <c r="E4" s="5" t="n"/>
+      <c r="F4" s="5" t="n"/>
+      <c r="G4" s="5" t="n"/>
+      <c r="H4" s="5" t="n"/>
+      <c r="I4" s="5" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" s="6" t="inlineStr">
+      <c r="A5" s="5" t="n"/>
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr"/>
-      <c r="D5" s="3" t="inlineStr"/>
-      <c r="E5" s="3" t="inlineStr"/>
-      <c r="F5" s="3" t="inlineStr"/>
-      <c r="G5" s="3" t="inlineStr"/>
-      <c r="H5" s="3" t="inlineStr"/>
-      <c r="I5" s="3" t="inlineStr"/>
+      <c r="C5" s="4" t="inlineStr"/>
+      <c r="D5" s="5" t="n"/>
+      <c r="E5" s="5" t="n"/>
+      <c r="F5" s="5" t="n"/>
+      <c r="G5" s="5" t="n"/>
+      <c r="H5" s="5" t="n"/>
+      <c r="I5" s="5" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="n"/>
+      <c r="B6" s="5" t="n"/>
+      <c r="C6" s="9" t="n"/>
+      <c r="D6" s="5" t="n"/>
+      <c r="E6" s="5" t="n"/>
+      <c r="F6" s="5" t="n"/>
+      <c r="G6" s="5" t="n"/>
+      <c r="H6" s="5" t="n"/>
+      <c r="I6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -597,63 +662,77 @@
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>CSE 1101 (Prof. H)</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>CSE 1100 (Prof. G)</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr"/>
-      <c r="F7" s="3" t="inlineStr"/>
-      <c r="G7" s="3" t="inlineStr"/>
-      <c r="H7" s="3" t="inlineStr"/>
-      <c r="I7" s="3" t="inlineStr"/>
+      <c r="E7" s="4" t="inlineStr"/>
+      <c r="F7" s="5" t="n"/>
+      <c r="G7" s="5" t="n"/>
+      <c r="H7" s="5" t="n"/>
+      <c r="I7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="4" t="inlineStr">
+      <c r="A8" s="5" t="n"/>
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr"/>
-      <c r="D8" s="3" t="inlineStr"/>
-      <c r="E8" s="3" t="inlineStr"/>
-      <c r="F8" s="3" t="inlineStr"/>
-      <c r="G8" s="3" t="inlineStr"/>
-      <c r="H8" s="3" t="inlineStr"/>
-      <c r="I8" s="3" t="inlineStr"/>
+      <c r="C8" s="4" t="inlineStr"/>
+      <c r="D8" s="5" t="n"/>
+      <c r="E8" s="5" t="n"/>
+      <c r="F8" s="5" t="n"/>
+      <c r="G8" s="5" t="n"/>
+      <c r="H8" s="5" t="n"/>
+      <c r="I8" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="B9" s="5" t="inlineStr">
+      <c r="A9" s="5" t="n"/>
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C9" s="3" t="inlineStr"/>
-      <c r="D9" s="3" t="inlineStr"/>
-      <c r="E9" s="3" t="inlineStr"/>
-      <c r="F9" s="3" t="inlineStr"/>
-      <c r="G9" s="3" t="inlineStr"/>
-      <c r="H9" s="3" t="inlineStr"/>
-      <c r="I9" s="3" t="inlineStr"/>
+      <c r="C9" s="4" t="inlineStr"/>
+      <c r="D9" s="5" t="n"/>
+      <c r="E9" s="5" t="n"/>
+      <c r="F9" s="5" t="n"/>
+      <c r="G9" s="5" t="n"/>
+      <c r="H9" s="5" t="n"/>
+      <c r="I9" s="5" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" s="6" t="inlineStr">
+      <c r="A10" s="5" t="n"/>
+      <c r="B10" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C10" s="3" t="inlineStr"/>
-      <c r="D10" s="3" t="inlineStr"/>
-      <c r="E10" s="3" t="inlineStr"/>
-      <c r="F10" s="3" t="inlineStr"/>
-      <c r="G10" s="3" t="inlineStr"/>
-      <c r="H10" s="3" t="inlineStr"/>
-      <c r="I10" s="3" t="inlineStr"/>
+      <c r="C10" s="4" t="inlineStr"/>
+      <c r="D10" s="5" t="n"/>
+      <c r="E10" s="5" t="n"/>
+      <c r="F10" s="5" t="n"/>
+      <c r="G10" s="5" t="n"/>
+      <c r="H10" s="5" t="n"/>
+      <c r="I10" s="5" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="n"/>
+      <c r="B11" s="5" t="n"/>
+      <c r="C11" s="9" t="n"/>
+      <c r="D11" s="5" t="n"/>
+      <c r="E11" s="5" t="n"/>
+      <c r="F11" s="5" t="n"/>
+      <c r="G11" s="5" t="n"/>
+      <c r="H11" s="5" t="n"/>
+      <c r="I11" s="5" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -666,63 +745,77 @@
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C12" s="3" t="inlineStr"/>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="C12" s="4" t="inlineStr"/>
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>CSE 1101 (Prof. H)</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
+      <c r="E12" s="3" t="inlineStr">
         <is>
           <t>CSE 1100 (Prof. G)</t>
         </is>
       </c>
-      <c r="F12" s="3" t="inlineStr"/>
-      <c r="G12" s="3" t="inlineStr"/>
-      <c r="H12" s="3" t="inlineStr"/>
-      <c r="I12" s="3" t="inlineStr"/>
+      <c r="F12" s="4" t="inlineStr"/>
+      <c r="G12" s="5" t="n"/>
+      <c r="H12" s="5" t="n"/>
+      <c r="I12" s="5" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="4" t="inlineStr">
+      <c r="A13" s="5" t="n"/>
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C13" s="3" t="inlineStr"/>
-      <c r="D13" s="3" t="inlineStr"/>
-      <c r="E13" s="3" t="inlineStr"/>
-      <c r="F13" s="3" t="inlineStr"/>
-      <c r="G13" s="3" t="inlineStr"/>
-      <c r="H13" s="3" t="inlineStr"/>
-      <c r="I13" s="3" t="inlineStr"/>
+      <c r="C13" s="4" t="inlineStr"/>
+      <c r="D13" s="5" t="n"/>
+      <c r="E13" s="5" t="n"/>
+      <c r="F13" s="5" t="n"/>
+      <c r="G13" s="5" t="n"/>
+      <c r="H13" s="5" t="n"/>
+      <c r="I13" s="5" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="5" t="inlineStr">
+      <c r="A14" s="5" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C14" s="3" t="inlineStr"/>
-      <c r="D14" s="3" t="inlineStr"/>
-      <c r="E14" s="3" t="inlineStr"/>
-      <c r="F14" s="3" t="inlineStr"/>
-      <c r="G14" s="3" t="inlineStr"/>
-      <c r="H14" s="3" t="inlineStr"/>
-      <c r="I14" s="3" t="inlineStr"/>
+      <c r="C14" s="4" t="inlineStr"/>
+      <c r="D14" s="5" t="n"/>
+      <c r="E14" s="5" t="n"/>
+      <c r="F14" s="5" t="n"/>
+      <c r="G14" s="5" t="n"/>
+      <c r="H14" s="5" t="n"/>
+      <c r="I14" s="5" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="6" t="inlineStr">
+      <c r="A15" s="5" t="n"/>
+      <c r="B15" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr"/>
-      <c r="D15" s="3" t="inlineStr"/>
-      <c r="E15" s="3" t="inlineStr"/>
-      <c r="F15" s="3" t="inlineStr"/>
-      <c r="G15" s="3" t="inlineStr"/>
-      <c r="H15" s="3" t="inlineStr"/>
-      <c r="I15" s="3" t="inlineStr"/>
+      <c r="C15" s="4" t="inlineStr"/>
+      <c r="D15" s="5" t="n"/>
+      <c r="E15" s="5" t="n"/>
+      <c r="F15" s="5" t="n"/>
+      <c r="G15" s="5" t="n"/>
+      <c r="H15" s="5" t="n"/>
+      <c r="I15" s="5" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="n"/>
+      <c r="B16" s="5" t="n"/>
+      <c r="C16" s="9" t="n"/>
+      <c r="D16" s="5" t="n"/>
+      <c r="E16" s="5" t="n"/>
+      <c r="F16" s="5" t="n"/>
+      <c r="G16" s="5" t="n"/>
+      <c r="H16" s="5" t="n"/>
+      <c r="I16" s="5" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -735,67 +828,77 @@
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C17" s="2" t="inlineStr">
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t>CSE 1104 (Prof. J)</t>
         </is>
       </c>
-      <c r="D17" s="2" t="inlineStr">
+      <c r="D17" s="3" t="inlineStr">
         <is>
           <t>CSE 1103 (Prof. I)</t>
         </is>
       </c>
-      <c r="E17" s="2" t="inlineStr">
-        <is>
-          <t>CSE 1103 (Prof. I)</t>
-        </is>
-      </c>
-      <c r="F17" s="3" t="inlineStr"/>
-      <c r="G17" s="3" t="inlineStr"/>
-      <c r="H17" s="3" t="inlineStr"/>
-      <c r="I17" s="3" t="inlineStr"/>
+      <c r="E17" s="5" t="n"/>
+      <c r="F17" s="4" t="inlineStr"/>
+      <c r="G17" s="5" t="n"/>
+      <c r="H17" s="5" t="n"/>
+      <c r="I17" s="5" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="4" t="inlineStr">
+      <c r="A18" s="5" t="n"/>
+      <c r="B18" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C18" s="3" t="inlineStr"/>
-      <c r="D18" s="3" t="inlineStr"/>
-      <c r="E18" s="3" t="inlineStr"/>
-      <c r="F18" s="3" t="inlineStr"/>
-      <c r="G18" s="3" t="inlineStr"/>
-      <c r="H18" s="3" t="inlineStr"/>
-      <c r="I18" s="3" t="inlineStr"/>
+      <c r="C18" s="4" t="inlineStr"/>
+      <c r="D18" s="5" t="n"/>
+      <c r="E18" s="5" t="n"/>
+      <c r="F18" s="5" t="n"/>
+      <c r="G18" s="5" t="n"/>
+      <c r="H18" s="5" t="n"/>
+      <c r="I18" s="5" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="5" t="inlineStr">
+      <c r="A19" s="5" t="n"/>
+      <c r="B19" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C19" s="3" t="inlineStr"/>
-      <c r="D19" s="3" t="inlineStr"/>
-      <c r="E19" s="3" t="inlineStr"/>
-      <c r="F19" s="3" t="inlineStr"/>
-      <c r="G19" s="3" t="inlineStr"/>
-      <c r="H19" s="3" t="inlineStr"/>
-      <c r="I19" s="3" t="inlineStr"/>
+      <c r="C19" s="4" t="inlineStr"/>
+      <c r="D19" s="5" t="n"/>
+      <c r="E19" s="5" t="n"/>
+      <c r="F19" s="5" t="n"/>
+      <c r="G19" s="5" t="n"/>
+      <c r="H19" s="5" t="n"/>
+      <c r="I19" s="5" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="6" t="inlineStr">
+      <c r="A20" s="5" t="n"/>
+      <c r="B20" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C20" s="3" t="inlineStr"/>
-      <c r="D20" s="3" t="inlineStr"/>
-      <c r="E20" s="3" t="inlineStr"/>
-      <c r="F20" s="3" t="inlineStr"/>
-      <c r="G20" s="3" t="inlineStr"/>
-      <c r="H20" s="3" t="inlineStr"/>
-      <c r="I20" s="3" t="inlineStr"/>
+      <c r="C20" s="4" t="inlineStr"/>
+      <c r="D20" s="5" t="n"/>
+      <c r="E20" s="5" t="n"/>
+      <c r="F20" s="5" t="n"/>
+      <c r="G20" s="5" t="n"/>
+      <c r="H20" s="5" t="n"/>
+      <c r="I20" s="5" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="n"/>
+      <c r="B21" s="5" t="n"/>
+      <c r="C21" s="9" t="n"/>
+      <c r="D21" s="5" t="n"/>
+      <c r="E21" s="5" t="n"/>
+      <c r="F21" s="5" t="n"/>
+      <c r="G21" s="5" t="n"/>
+      <c r="H21" s="5" t="n"/>
+      <c r="I21" s="5" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -808,71 +911,99 @@
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C22" s="3" t="inlineStr"/>
-      <c r="D22" s="2" t="inlineStr">
+      <c r="C22" s="4" t="inlineStr"/>
+      <c r="D22" s="3" t="inlineStr">
         <is>
           <t>CSE 1104 (Prof. J)</t>
         </is>
       </c>
-      <c r="E22" s="2" t="inlineStr">
+      <c r="E22" s="3" t="inlineStr">
         <is>
           <t>CSE 1103 (Prof. I)</t>
         </is>
       </c>
-      <c r="F22" s="3" t="inlineStr"/>
-      <c r="G22" s="3" t="inlineStr"/>
-      <c r="H22" s="3" t="inlineStr"/>
-      <c r="I22" s="3" t="inlineStr"/>
+      <c r="F22" s="4" t="inlineStr"/>
+      <c r="G22" s="5" t="n"/>
+      <c r="H22" s="5" t="n"/>
+      <c r="I22" s="5" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="4" t="inlineStr">
+      <c r="A23" s="5" t="n"/>
+      <c r="B23" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C23" s="3" t="inlineStr"/>
-      <c r="D23" s="3" t="inlineStr"/>
-      <c r="E23" s="3" t="inlineStr"/>
-      <c r="F23" s="3" t="inlineStr"/>
-      <c r="G23" s="3" t="inlineStr"/>
-      <c r="H23" s="3" t="inlineStr"/>
-      <c r="I23" s="3" t="inlineStr"/>
+      <c r="C23" s="4" t="inlineStr"/>
+      <c r="D23" s="5" t="n"/>
+      <c r="E23" s="5" t="n"/>
+      <c r="F23" s="5" t="n"/>
+      <c r="G23" s="5" t="n"/>
+      <c r="H23" s="5" t="n"/>
+      <c r="I23" s="5" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="5" t="inlineStr">
+      <c r="A24" s="5" t="n"/>
+      <c r="B24" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C24" s="3" t="inlineStr"/>
-      <c r="D24" s="3" t="inlineStr"/>
-      <c r="E24" s="3" t="inlineStr"/>
-      <c r="F24" s="3" t="inlineStr"/>
-      <c r="G24" s="3" t="inlineStr"/>
-      <c r="H24" s="3" t="inlineStr"/>
-      <c r="I24" s="3" t="inlineStr"/>
+      <c r="C24" s="4" t="inlineStr"/>
+      <c r="D24" s="5" t="n"/>
+      <c r="E24" s="5" t="n"/>
+      <c r="F24" s="5" t="n"/>
+      <c r="G24" s="5" t="n"/>
+      <c r="H24" s="5" t="n"/>
+      <c r="I24" s="5" t="n"/>
     </row>
     <row r="25">
-      <c r="B25" s="6" t="inlineStr">
+      <c r="A25" s="5" t="n"/>
+      <c r="B25" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C25" s="3" t="inlineStr"/>
-      <c r="D25" s="3" t="inlineStr"/>
-      <c r="E25" s="3" t="inlineStr"/>
-      <c r="F25" s="3" t="inlineStr"/>
-      <c r="G25" s="3" t="inlineStr"/>
-      <c r="H25" s="3" t="inlineStr"/>
-      <c r="I25" s="3" t="inlineStr"/>
+      <c r="C25" s="4" t="inlineStr"/>
+      <c r="D25" s="5" t="n"/>
+      <c r="E25" s="5" t="n"/>
+      <c r="F25" s="5" t="n"/>
+      <c r="G25" s="5" t="n"/>
+      <c r="H25" s="5" t="n"/>
+      <c r="I25" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="30">
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C18:I18"/>
     <mergeCell ref="A7:A10"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C14:I14"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C25:I25"/>
     <mergeCell ref="A22:A25"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="F22:I22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
lab classes logic updated
</commit_message>
<xml_diff>
--- a/routine_final.xlsx
+++ b/routine_final.xlsx
@@ -64,7 +64,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,40 +78,15 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -124,7 +99,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -134,7 +108,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -532,478 +506,930 @@
           <t>Year</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>9:00-10:00</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>10:00-11:00</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>11:00-12:00</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>12:00-1:00</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>2:00-3:00</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>3:00-4:00</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>4:00-5:00</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1100 (Prof. G)</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="inlineStr"/>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1101 (Prof. H)</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr"/>
-      <c r="G2" s="5" t="n"/>
-      <c r="H2" s="5" t="n"/>
-      <c r="I2" s="5" t="n"/>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1101 (Prof. G)</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1105 (Prof. J)</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1103 (Prof. I)</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1104 (Prof. A)</t>
+        </is>
+      </c>
+      <c r="H2" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1102 (Prof. H)</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n"/>
       <c r="B3" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr"/>
-      <c r="D3" s="5" t="n"/>
-      <c r="E3" s="5" t="n"/>
-      <c r="F3" s="5" t="n"/>
-      <c r="G3" s="5" t="n"/>
-      <c r="H3" s="5" t="n"/>
-      <c r="I3" s="5" t="n"/>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n"/>
       <c r="B4" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr"/>
-      <c r="D4" s="5" t="n"/>
-      <c r="E4" s="5" t="n"/>
-      <c r="F4" s="5" t="n"/>
-      <c r="G4" s="5" t="n"/>
-      <c r="H4" s="5" t="n"/>
-      <c r="I4" s="5" t="n"/>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n"/>
       <c r="B5" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr"/>
-      <c r="D5" s="5" t="n"/>
-      <c r="E5" s="5" t="n"/>
-      <c r="F5" s="5" t="n"/>
-      <c r="G5" s="5" t="n"/>
-      <c r="H5" s="5" t="n"/>
-      <c r="I5" s="5" t="n"/>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n"/>
-      <c r="B6" s="5" t="n"/>
       <c r="C6" s="9" t="n"/>
-      <c r="D6" s="5" t="n"/>
-      <c r="E6" s="5" t="n"/>
-      <c r="F6" s="5" t="n"/>
-      <c r="G6" s="5" t="n"/>
-      <c r="H6" s="5" t="n"/>
-      <c r="I6" s="5" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Monday</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1101 (Prof. H)</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1100 (Prof. G)</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="inlineStr"/>
-      <c r="F7" s="5" t="n"/>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="5" t="n"/>
-      <c r="I7" s="5" t="n"/>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1107 (Prof. C)</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1101 (Prof. G)</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1109 (Prof. E)</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1103 (Prof. I)</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="n"/>
       <c r="B8" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr"/>
-      <c r="D8" s="5" t="n"/>
-      <c r="E8" s="5" t="n"/>
-      <c r="F8" s="5" t="n"/>
-      <c r="G8" s="5" t="n"/>
-      <c r="H8" s="5" t="n"/>
-      <c r="I8" s="5" t="n"/>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr"/>
-      <c r="D9" s="5" t="n"/>
-      <c r="E9" s="5" t="n"/>
-      <c r="F9" s="5" t="n"/>
-      <c r="G9" s="5" t="n"/>
-      <c r="H9" s="5" t="n"/>
-      <c r="I9" s="5" t="n"/>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E9" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F9" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="n"/>
       <c r="B10" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr"/>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
-      <c r="I10" s="5" t="n"/>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n"/>
-      <c r="B11" s="5" t="n"/>
       <c r="C11" s="9" t="n"/>
-      <c r="D11" s="5" t="n"/>
-      <c r="E11" s="5" t="n"/>
-      <c r="F11" s="5" t="n"/>
-      <c r="G11" s="5" t="n"/>
-      <c r="H11" s="5" t="n"/>
-      <c r="I11" s="5" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="B12" s="2" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C12" s="4" t="inlineStr"/>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1101 (Prof. H)</t>
-        </is>
-      </c>
-      <c r="E12" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1100 (Prof. G)</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="inlineStr"/>
-      <c r="G12" s="5" t="n"/>
-      <c r="H12" s="5" t="n"/>
-      <c r="I12" s="5" t="n"/>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1103 (Prof. I)</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1107 (Prof. C)</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1101 (Prof. G)</t>
+        </is>
+      </c>
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1109 (Prof. E)</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1110 (Prof. F)</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="n"/>
       <c r="B13" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C13" s="4" t="inlineStr"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
-      <c r="I13" s="5" t="n"/>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="n"/>
       <c r="B14" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C14" s="4" t="inlineStr"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
-      <c r="I14" s="5" t="n"/>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="n"/>
       <c r="B15" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C15" s="4" t="inlineStr"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
-      <c r="I15" s="5" t="n"/>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F15" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="n"/>
-      <c r="B16" s="5" t="n"/>
       <c r="C16" s="9" t="n"/>
-      <c r="D16" s="5" t="n"/>
-      <c r="E16" s="5" t="n"/>
-      <c r="F16" s="5" t="n"/>
-      <c r="G16" s="5" t="n"/>
-      <c r="H16" s="5" t="n"/>
-      <c r="I16" s="5" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="B17" s="2" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
         <is>
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1104 (Prof. J)</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1103 (Prof. I)</t>
-        </is>
-      </c>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="4" t="inlineStr"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
-      <c r="I17" s="5" t="n"/>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1105 (Prof. J)</t>
+        </is>
+      </c>
+      <c r="F17" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1107 (Prof. C)</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1106 (Prof. B)</t>
+        </is>
+      </c>
+      <c r="H17" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="n"/>
       <c r="B18" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C18" s="4" t="inlineStr"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
-      <c r="I18" s="5" t="n"/>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="n"/>
       <c r="B19" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C19" s="4" t="inlineStr"/>
-      <c r="D19" s="5" t="n"/>
-      <c r="E19" s="5" t="n"/>
-      <c r="F19" s="5" t="n"/>
-      <c r="G19" s="5" t="n"/>
-      <c r="H19" s="5" t="n"/>
-      <c r="I19" s="5" t="n"/>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="n"/>
       <c r="B20" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C20" s="4" t="inlineStr"/>
-      <c r="D20" s="5" t="n"/>
-      <c r="E20" s="5" t="n"/>
-      <c r="F20" s="5" t="n"/>
-      <c r="G20" s="5" t="n"/>
-      <c r="H20" s="5" t="n"/>
-      <c r="I20" s="5" t="n"/>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="n"/>
-      <c r="B21" s="5" t="n"/>
       <c r="C21" s="9" t="n"/>
-      <c r="D21" s="5" t="n"/>
-      <c r="E21" s="5" t="n"/>
-      <c r="F21" s="5" t="n"/>
-      <c r="G21" s="5" t="n"/>
-      <c r="H21" s="5" t="n"/>
-      <c r="I21" s="5" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>Thursday</t>
         </is>
       </c>
-      <c r="B22" s="2" t="inlineStr">
+      <c r="B22" s="3" t="inlineStr">
         <is>
           <t>1st Year</t>
         </is>
       </c>
-      <c r="C22" s="4" t="inlineStr"/>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1104 (Prof. J)</t>
-        </is>
-      </c>
-      <c r="E22" s="3" t="inlineStr">
-        <is>
-          <t>CSE 1103 (Prof. I)</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="inlineStr"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
-      <c r="I22" s="5" t="n"/>
+      <c r="C22" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1109 (Prof. E)</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>CSE 1108 (Prof. D)</t>
+        </is>
+      </c>
+      <c r="H22" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="n"/>
       <c r="B23" s="6" t="inlineStr">
         <is>
           <t>2nd Year</t>
         </is>
       </c>
-      <c r="C23" s="4" t="inlineStr"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
-      <c r="I23" s="5" t="n"/>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="n"/>
       <c r="B24" s="7" t="inlineStr">
         <is>
           <t>3rd Year</t>
         </is>
       </c>
-      <c r="C24" s="4" t="inlineStr"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
-      <c r="I24" s="5" t="n"/>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F24" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="n"/>
       <c r="B25" s="8" t="inlineStr">
         <is>
           <t>4th Year</t>
         </is>
       </c>
-      <c r="C25" s="4" t="inlineStr"/>
-      <c r="D25" s="5" t="n"/>
-      <c r="E25" s="5" t="n"/>
-      <c r="F25" s="5" t="n"/>
-      <c r="G25" s="5" t="n"/>
-      <c r="H25" s="5" t="n"/>
-      <c r="I25" s="5" t="n"/>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H25" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C18:I18"/>
+  <mergeCells count="9">
     <mergeCell ref="A7:A10"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C14:I14"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A17:A20"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C6:I6"/>
     <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C11:I11"/>
     <mergeCell ref="A22:A25"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="F22:I22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>